<commit_message>
Tweaked the reader functions to remove read_csvs integer interpretation and adjusted tests and samples accordingly. Also augmented the samples and conftest data to include a 0 padded numeric value stored as text.
</commit_message>
<xml_diff>
--- a/tests/samples/excel/simple.xlsx
+++ b/tests/samples/excel/simple.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -57,6 +57,21 @@
   </si>
   <si>
     <t>Soto</t>
+  </si>
+  <si>
+    <t>foreign_key</t>
+  </si>
+  <si>
+    <t>00025</t>
+  </si>
+  <si>
+    <t>00076</t>
+  </si>
+  <si>
+    <t>00123</t>
+  </si>
+  <si>
+    <t>01234</t>
   </si>
 </sst>
 </file>
@@ -92,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,15 +390,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,8 +411,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -403,8 +425,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -414,8 +439,11 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -425,8 +453,11 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -435,6 +466,9 @@
       </c>
       <c r="C5" t="s">
         <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>